<commit_message>
Update mcode to 0.9
</commit_message>
<xml_diff>
--- a/docs/mcode/onco-core-CancerCondition.xlsx
+++ b/docs/mcode/onco-core-CancerCondition.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$57</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1544" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="325">
   <si>
     <t>Path</t>
   </si>
@@ -506,7 +506,10 @@
     <t>preferred</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/mcode/shr/core/vs/ConditionCategoryVS</t>
+    <t>Extended category code valueset to support the intent of the separate concepts of problems and health concerns</t>
+  </si>
+  <si>
+    <t>http://fhir.org/guides/argonaut/ValueSet/condition-category</t>
   </si>
   <si>
     <t>'problem' if from PRB-3. 'diagnosis' if from DG1 segment in PV1 message</t>
@@ -516,6 +519,196 @@
   </si>
   <si>
     <t>class</t>
+  </si>
+  <si>
+    <t>Condition.category.id</t>
+  </si>
+  <si>
+    <t>xml:id (or equivalent in JSON)</t>
+  </si>
+  <si>
+    <t>unique id for the element within a resource (for internal references).</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Condition.category.extension</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. In order to make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>Condition.category.coding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coding {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>Code defined by a terminology system</t>
+  </si>
+  <si>
+    <t>A reference to a code defined by a terminology system.</t>
+  </si>
+  <si>
+    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labelled as UserSelected = true.</t>
+  </si>
+  <si>
+    <t>Allows for translations and alternate encodings within a code system.  Also supports communication of the same instance to systems requiring different encodings.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:code}
+</t>
+  </si>
+  <si>
+    <t>C*E.1-8, C*E.10-22</t>
+  </si>
+  <si>
+    <t>union(., ./translation)</t>
+  </si>
+  <si>
+    <t>Fixed_64572001</t>
+  </si>
+  <si>
+    <t>Disease</t>
+  </si>
+  <si>
+    <t>Condition.category.coding.id</t>
+  </si>
+  <si>
+    <t>Condition.category.coding.extension</t>
+  </si>
+  <si>
+    <t>Condition.category.coding.system</t>
+  </si>
+  <si>
+    <t>Identity of the terminology system</t>
+  </si>
+  <si>
+    <t>The identification of the code system that defines the meaning of the symbol in the code.</t>
+  </si>
+  <si>
+    <t>The URI may be an OID (urn:oid:...) or a UUID (urn:uuid:...).  OIDs and UUIDs SHALL be references to the HL7 OID registry. Otherwise, the URI should come from HL7's list of FHIR defined special URIs or it should de-reference to some definition that establish the system clearly and unambiguously.</t>
+  </si>
+  <si>
+    <t>Need to be unambiguous about the source of the definition of the symbol.</t>
+  </si>
+  <si>
+    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://snomed.info/sct"/&gt;</t>
+  </si>
+  <si>
+    <t>C*E.3</t>
+  </si>
+  <si>
+    <t>./codeSystem</t>
+  </si>
+  <si>
+    <t>Condition.category.coding.version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>Version of the system - if relevant</t>
+  </si>
+  <si>
+    <t>The version of the code system which was used when choosing this code. Note that a well-maintained code system does not need the version reported, because the meaning of codes is consistent across versions. However this cannot consistently be assured. and when the meaning is not guaranteed to be consistent, the version SHOULD be exchanged.</t>
+  </si>
+  <si>
+    <t>Where the terminology does not clearly define what string should be used to identify code system versions, the recommendation is to use the date (expressed in FHIR date format) on which that version was officially published as the version date.</t>
+  </si>
+  <si>
+    <t>C*E.7</t>
+  </si>
+  <si>
+    <t>./codeSystemVersion</t>
+  </si>
+  <si>
+    <t>Condition.category.coding.code</t>
+  </si>
+  <si>
+    <t>Symbol in syntax defined by the system</t>
+  </si>
+  <si>
+    <t>A symbol in syntax defined by the system. The symbol may be a predefined code or an expression in a syntax defined by the coding system (e.g. post-coordination).</t>
+  </si>
+  <si>
+    <t>Need to refer to a particular code in the system.</t>
+  </si>
+  <si>
+    <t>&lt;valueCode xmlns="http://hl7.org/fhir" value="64572001"/&gt;</t>
+  </si>
+  <si>
+    <t>C*E.1</t>
+  </si>
+  <si>
+    <t>./code</t>
+  </si>
+  <si>
+    <t>Condition.category.coding.display</t>
+  </si>
+  <si>
+    <t>Representation defined by the system</t>
+  </si>
+  <si>
+    <t>A representation of the meaning of the code in the system, following the rules of the system.</t>
+  </si>
+  <si>
+    <t>Need to be able to carry a human-readable meaning of the code for readers that do not know  the system.</t>
+  </si>
+  <si>
+    <t>C*E.2 - but note this is not well followed</t>
+  </si>
+  <si>
+    <t>CV.displayName</t>
+  </si>
+  <si>
+    <t>Condition.category.coding.userSelected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boolean {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>If this coding was chosen directly by the user</t>
+  </si>
+  <si>
+    <t>Indicates that this coding was chosen by a user directly - i.e. off a pick list of available items (codes or displays).</t>
+  </si>
+  <si>
+    <t>Amongst a set of alternatives, a directly chosen code is the most appropriate starting point for new translations. There is some ambiguity about what exactly 'directly chosen' implies, and trading partner agreement may be needed to clarify the use of this element and its consequences more completely.</t>
+  </si>
+  <si>
+    <t>This has been identified as a clinical safety criterium - that this exact system/code pair was chosen explicitly, rather than inferred by the system based on some rules or language processing.</t>
+  </si>
+  <si>
+    <t>Sometimes implied by being first</t>
+  </si>
+  <si>
+    <t>CD.codingRationale</t>
+  </si>
+  <si>
+    <t>Condition.category.text</t>
+  </si>
+  <si>
+    <t>Plain text representation of the concept</t>
+  </si>
+  <si>
+    <t>A human language representation of the concept as seen/selected/uttered by the user who entered the data and/or which represents the intended meaning of the user.</t>
+  </si>
+  <si>
+    <t>Very often the text is the same as a displayName of one of the codings.</t>
+  </si>
+  <si>
+    <t>The codes from the terminologies do not always capture the correct meaning with all the nuances of the human using them, or sometimes there is no appropriate code at all. In these cases, the text is used to capture the full meaning of the source.</t>
+  </si>
+  <si>
+    <t>C*E.9. But note many systems use C*E.2 for this</t>
+  </si>
+  <si>
+    <t>./originalText[mediaType/code="text/plain"]/data</t>
   </si>
   <si>
     <t>Condition.clinicalStatus</t>
@@ -648,19 +841,7 @@
     <t>Condition.stage.id</t>
   </si>
   <si>
-    <t>xml:id (or equivalent in JSON)</t>
-  </si>
-  <si>
-    <t>unique id for the element within a resource (for internal references).</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>Condition.stage.extension</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. In order to make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
   </si>
   <si>
     <t>Condition.stage.modifierExtension</t>
@@ -806,7 +987,7 @@
   </si>
   <si>
     <t>Body side of the body location, if needed to distinguish from a similar location on the other side of the body.
-This extension is part of the profile on body site appearing throughout the mCODE implementation guide. Body location is a flexible structure that allows the location to be determined by a single code, or a code plus laterality and/or orientation. The body location can also be specified in relation to one or more body landmarks. SNOMED CT is used in all cases.
+The laterality element is part of BodyLocation, a flexible structure that allows the location to be determined by a single code, or a code plus laterality and/or orientation. The body location can also be specified in relation to one or more body landmarks. SNOMED CT is used in all cases.
 + Code only: The code should include (precoordinate) laterality and/orientation to the degree necessary to completely specify the body location.
 + Code plus laterality and/or orientation: The basic code augmented by codes specifying the body side and/or anatomical orientation.
 + Relation to landmark: The location relative to a landmark is specified by:
@@ -823,7 +1004,7 @@
   </si>
   <si>
     <t>Orientation of the body location, if needed to distinguish from a similar location in another orientation.
-This extension is part of the profile on body site appearing throughout the mCODE implementation guide. Body location is a flexible structure that allows the location to be determined by a single code, or a code plus laterality and/or orientation. The body location can also be specified in relation to one or more body landmarks. SNOMED CT is used in all cases.
+The orientation element is part of BodyLocation, a flexible structure that allows the location to be determined by a single code, or a code plus laterality and/or orientation. The body location can also be specified in relation to one or more body landmarks. SNOMED CT is used in all cases.
 + Code only: The code should include (precoordinate) laterality and/orientation to the degree necessary to completely specify the body location.
 + Code plus laterality and/or orientation: The basic code augmented by codes specifying the body side and/or anatomical orientation.
 + Relation to landmark: The location relative to a landmark is specified by:
@@ -843,7 +1024,7 @@
 * Specifying the location and type of landmark using a body site code and optional laterality/orientation,
 * Specifying the direction from the landmark to the body location, and
 * Specifying the distance from the landmark to the body location.
-This extension is part of the profile on body site appearing throughout the mCODE implementation guide. Body location is a flexible structure that allows the location to be determined by a single code, or a code plus laterality and/or orientation. The body location can also be specified in relation to one or more body landmarks. SNOMED CT is used in all cases.
+The RelationToLandmark element is part of BodyLocation, a flexible structure that allows the location to be determined by a single code, or a code plus laterality and/or orientation. The body location can also be specified in relation to one or more body landmarks. SNOMED CT is used in all cases.
 + Code only: The code should include (precoordinate) laterality and/orientation to the degree necessary to completely specify the body location.
 + Code plus laterality and/or orientation: The basic code augmented by codes specifying the body side and/or anatomical orientation.
 + Relation to landmark: The location relative to a landmark is specified by:
@@ -855,51 +1036,7 @@
     <t>Condition.bodySite.coding</t>
   </si>
   <si>
-    <t xml:space="preserve">Coding {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>Code defined by a terminology system</t>
-  </si>
-  <si>
-    <t>A reference to a code defined by a terminology system.</t>
-  </si>
-  <si>
-    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labelled as UserSelected = true.</t>
-  </si>
-  <si>
-    <t>Allows for translations and alternate encodings within a code system.  Also supports communication of the same instance to systems requiring different encodings.</t>
-  </si>
-  <si>
-    <t>C*E.1-8, C*E.10-22</t>
-  </si>
-  <si>
-    <t>union(., ./translation)</t>
-  </si>
-  <si>
     <t>Condition.bodySite.text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>Plain text representation of the concept</t>
-  </si>
-  <si>
-    <t>A human language representation of the concept as seen/selected/uttered by the user who entered the data and/or which represents the intended meaning of the user.</t>
-  </si>
-  <si>
-    <t>Very often the text is the same as a displayName of one of the codings.</t>
-  </si>
-  <si>
-    <t>The codes from the terminologies do not always capture the correct meaning with all the nuances of the human using them, or sometimes there is no appropriate code at all. In these cases, the text is used to capture the full meaning of the source.</t>
-  </si>
-  <si>
-    <t>C*E.9. But note many systems use C*E.2 for this</t>
-  </si>
-  <si>
-    <t>./originalText[mediaType/code="text/plain"]/data</t>
   </si>
   <si>
     <t>Condition.notes</t>
@@ -1063,7 +1200,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN45"/>
+  <dimension ref="A1:AN57"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1072,7 +1209,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="35.19140625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="36.625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="27.890625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
@@ -1095,7 +1232,7 @@
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="77.01171875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="102.35546875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="61.34765625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
@@ -3163,9 +3300,11 @@
       <c r="W19" t="s" s="2">
         <v>155</v>
       </c>
-      <c r="X19" s="2"/>
+      <c r="X19" t="s" s="2">
+        <v>156</v>
+      </c>
       <c r="Y19" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="Z19" t="s" s="2">
         <v>40</v>
@@ -3201,18 +3340,18 @@
         <v>151</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3220,28 +3359,28 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F20" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H20" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I20" t="s" s="2">
         <v>40</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -3265,14 +3404,16 @@
         <v>40</v>
       </c>
       <c r="V20" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W20" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="X20" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="X20" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Y20" t="s" s="2">
-        <v>163</v>
+        <v>40</v>
       </c>
       <c r="Z20" t="s" s="2">
         <v>40</v>
@@ -3289,15 +3430,11 @@
       <c r="AD20" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AE20" t="s" s="2">
-        <v>160</v>
-      </c>
+      <c r="AE20" s="2"/>
       <c r="AF20" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AG20" t="s" s="2">
-        <v>50</v>
-      </c>
+      <c r="AG20" s="2"/>
       <c r="AH20" t="s" s="2">
         <v>40</v>
       </c>
@@ -3305,52 +3442,54 @@
         <v>40</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>160</v>
+        <v>40</v>
       </c>
       <c r="AK20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL20" t="s" s="2">
         <v>164</v>
       </c>
-      <c r="AL20" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="AM20" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" hidden="true">
+      <c r="A21" t="s" s="2">
         <v>165</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="2">
-        <v>166</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H21" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I21" t="s" s="2">
         <v>40</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>167</v>
+        <v>91</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="M21" s="2"/>
+        <v>166</v>
+      </c>
+      <c r="M21" t="s" s="2">
+        <v>93</v>
+      </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
         <v>40</v>
@@ -3372,14 +3511,16 @@
         <v>40</v>
       </c>
       <c r="V21" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="X21" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="X21" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Y21" t="s" s="2">
-        <v>169</v>
+        <v>40</v>
       </c>
       <c r="Z21" t="s" s="2">
         <v>40</v>
@@ -3396,15 +3537,11 @@
       <c r="AD21" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AE21" t="s" s="2">
-        <v>166</v>
-      </c>
+      <c r="AE21" s="2"/>
       <c r="AF21" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AG21" t="s" s="2">
-        <v>50</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="AG21" s="2"/>
       <c r="AH21" t="s" s="2">
         <v>40</v>
       </c>
@@ -3412,21 +3549,21 @@
         <v>40</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>166</v>
+        <v>40</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>170</v>
+        <v>40</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>165</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3434,10 +3571,10 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>40</v>
@@ -3449,18 +3586,20 @@
         <v>51</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>175</v>
-      </c>
-      <c r="N22" s="2"/>
+        <v>171</v>
+      </c>
+      <c r="N22" t="s" s="2">
+        <v>172</v>
+      </c>
       <c r="O22" t="s" s="2">
         <v>40</v>
       </c>
@@ -3481,71 +3620,67 @@
         <v>40</v>
       </c>
       <c r="V22" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="X22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA22" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="AB22" s="2"/>
+      <c r="AC22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD22" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AE22" s="2"/>
+      <c r="AF22" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG22" s="2"/>
+      <c r="AH22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK22" t="s" s="2">
         <v>174</v>
       </c>
-      <c r="Y22" t="s" s="2">
-        <v>176</v>
-      </c>
-      <c r="Z22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE22" t="s" s="2">
-        <v>172</v>
-      </c>
-      <c r="AF22" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG22" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK22" t="s" s="2">
-        <v>177</v>
-      </c>
       <c r="AL22" t="s" s="2">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>179</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>180</v>
-      </c>
-      <c r="B23" s="2"/>
+        <v>167</v>
+      </c>
+      <c r="B23" t="s" s="2">
+        <v>176</v>
+      </c>
       <c r="C23" t="s" s="2">
         <v>40</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F23" t="s" s="2">
         <v>50</v>
@@ -3560,17 +3695,15 @@
         <v>51</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>184</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>40</v>
@@ -3592,7 +3725,7 @@
         <v>40</v>
       </c>
       <c r="V23" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W23" t="s" s="2">
         <v>40</v>
@@ -3618,15 +3751,11 @@
       <c r="AD23" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AE23" t="s" s="2">
-        <v>180</v>
-      </c>
+      <c r="AE23" s="2"/>
       <c r="AF23" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AG23" t="s" s="2">
-        <v>50</v>
-      </c>
+      <c r="AG23" s="2"/>
       <c r="AH23" t="s" s="2">
         <v>40</v>
       </c>
@@ -3637,18 +3766,18 @@
         <v>40</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>185</v>
+        <v>40</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>186</v>
+        <v>40</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>187</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3668,20 +3797,18 @@
         <v>40</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>189</v>
+        <v>52</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>192</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
         <v>40</v>
@@ -3703,7 +3830,7 @@
         <v>40</v>
       </c>
       <c r="V24" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W24" t="s" s="2">
         <v>40</v>
@@ -3729,15 +3856,11 @@
       <c r="AD24" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AE24" t="s" s="2">
-        <v>188</v>
-      </c>
+      <c r="AE24" s="2"/>
       <c r="AF24" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AG24" t="s" s="2">
-        <v>50</v>
-      </c>
+      <c r="AG24" s="2"/>
       <c r="AH24" t="s" s="2">
         <v>40</v>
       </c>
@@ -3751,26 +3874,26 @@
         <v>40</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>193</v>
+        <v>164</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>194</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G25" t="s" s="2">
         <v>40</v>
@@ -3779,18 +3902,20 @@
         <v>40</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>196</v>
+        <v>90</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>197</v>
+        <v>91</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="M25" s="2"/>
+        <v>166</v>
+      </c>
+      <c r="M25" t="s" s="2">
+        <v>93</v>
+      </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
         <v>40</v>
@@ -3812,7 +3937,7 @@
         <v>40</v>
       </c>
       <c r="V25" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W25" t="s" s="2">
         <v>40</v>
@@ -3838,20 +3963,16 @@
       <c r="AD25" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AE25" t="s" s="2">
-        <v>195</v>
-      </c>
+      <c r="AE25" s="2"/>
       <c r="AF25" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AG25" t="s" s="2">
-        <v>50</v>
-      </c>
+      <c r="AG25" s="2"/>
       <c r="AH25" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>199</v>
+        <v>40</v>
       </c>
       <c r="AJ25" t="s" s="2">
         <v>40</v>
@@ -3860,7 +3981,7 @@
         <v>40</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>200</v>
+        <v>164</v>
       </c>
       <c r="AM25" t="s" s="2">
         <v>40</v>
@@ -3868,7 +3989,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3888,25 +4009,29 @@
         <v>40</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="M26" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="N26" t="s" s="2">
+        <v>184</v>
+      </c>
       <c r="O26" t="s" s="2">
         <v>40</v>
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" t="s" s="2">
-        <v>40</v>
+        <v>185</v>
       </c>
       <c r="R26" t="s" s="2">
         <v>40</v>
@@ -3921,7 +4046,7 @@
         <v>40</v>
       </c>
       <c r="V26" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W26" t="s" s="2">
         <v>40</v>
@@ -3947,15 +4072,11 @@
       <c r="AD26" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AE26" t="s" s="2">
-        <v>201</v>
-      </c>
+      <c r="AE26" s="2"/>
       <c r="AF26" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AG26" t="s" s="2">
-        <v>50</v>
-      </c>
+      <c r="AG26" s="2"/>
       <c r="AH26" t="s" s="2">
         <v>40</v>
       </c>
@@ -3966,10 +4087,10 @@
         <v>40</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>40</v>
+        <v>186</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="AM26" t="s" s="2">
         <v>40</v>
@@ -3977,18 +4098,18 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>40</v>
@@ -3997,19 +4118,19 @@
         <v>40</v>
       </c>
       <c r="I27" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>90</v>
+        <v>189</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>91</v>
+        <v>190</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>93</v>
+        <v>192</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
@@ -4032,7 +4153,7 @@
         <v>40</v>
       </c>
       <c r="V27" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W27" t="s" s="2">
         <v>40</v>
@@ -4058,15 +4179,11 @@
       <c r="AD27" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AE27" t="s" s="2">
-        <v>205</v>
-      </c>
+      <c r="AE27" s="2"/>
       <c r="AF27" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AG27" t="s" s="2">
-        <v>42</v>
-      </c>
+      <c r="AG27" s="2"/>
       <c r="AH27" t="s" s="2">
         <v>40</v>
       </c>
@@ -4077,10 +4194,10 @@
         <v>40</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>40</v>
+        <v>193</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>40</v>
@@ -4088,47 +4205,47 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
-        <v>208</v>
+        <v>40</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I28" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="I28" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J28" t="s" s="2">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>103</v>
+        <v>196</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="N28" s="2"/>
+        <v>197</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" t="s" s="2">
+        <v>198</v>
+      </c>
       <c r="O28" t="s" s="2">
         <v>40</v>
       </c>
       <c r="P28" s="2"/>
       <c r="Q28" t="s" s="2">
-        <v>40</v>
+        <v>199</v>
       </c>
       <c r="R28" t="s" s="2">
         <v>40</v>
@@ -4143,7 +4260,7 @@
         <v>40</v>
       </c>
       <c r="V28" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W28" t="s" s="2">
         <v>40</v>
@@ -4169,15 +4286,11 @@
       <c r="AD28" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AE28" t="s" s="2">
-        <v>207</v>
-      </c>
+      <c r="AE28" s="2"/>
       <c r="AF28" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AG28" t="s" s="2">
-        <v>42</v>
-      </c>
+      <c r="AG28" s="2"/>
       <c r="AH28" t="s" s="2">
         <v>40</v>
       </c>
@@ -4188,10 +4301,10 @@
         <v>40</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>87</v>
+        <v>201</v>
       </c>
       <c r="AM28" t="s" s="2">
         <v>40</v>
@@ -4199,7 +4312,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4222,16 +4335,18 @@
         <v>51</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>143</v>
+        <v>189</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
+      <c r="N29" t="s" s="2">
+        <v>205</v>
+      </c>
       <c r="O29" t="s" s="2">
         <v>40</v>
       </c>
@@ -4252,16 +4367,16 @@
         <v>40</v>
       </c>
       <c r="V29" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>213</v>
+        <v>40</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>214</v>
+        <v>40</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>215</v>
+        <v>40</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>40</v>
@@ -4278,17 +4393,13 @@
       <c r="AD29" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AE29" t="s" s="2">
-        <v>210</v>
-      </c>
+      <c r="AE29" s="2"/>
       <c r="AF29" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AG29" t="s" s="2">
-        <v>50</v>
-      </c>
+      <c r="AG29" s="2"/>
       <c r="AH29" t="s" s="2">
-        <v>216</v>
+        <v>40</v>
       </c>
       <c r="AI29" t="s" s="2">
         <v>40</v>
@@ -4297,10 +4408,10 @@
         <v>40</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>149</v>
+        <v>207</v>
       </c>
       <c r="AM29" t="s" s="2">
         <v>40</v>
@@ -4308,7 +4419,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4331,16 +4442,20 @@
         <v>51</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+        <v>211</v>
+      </c>
+      <c r="M30" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="N30" t="s" s="2">
+        <v>213</v>
+      </c>
       <c r="O30" t="s" s="2">
         <v>40</v>
       </c>
@@ -4361,7 +4476,7 @@
         <v>40</v>
       </c>
       <c r="V30" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W30" t="s" s="2">
         <v>40</v>
@@ -4387,17 +4502,13 @@
       <c r="AD30" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AE30" t="s" s="2">
-        <v>218</v>
-      </c>
+      <c r="AE30" s="2"/>
       <c r="AF30" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AG30" t="s" s="2">
-        <v>42</v>
-      </c>
+      <c r="AG30" s="2"/>
       <c r="AH30" t="s" s="2">
-        <v>216</v>
+        <v>40</v>
       </c>
       <c r="AI30" t="s" s="2">
         <v>40</v>
@@ -4406,10 +4517,10 @@
         <v>40</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>40</v>
+        <v>214</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="AM30" t="s" s="2">
         <v>40</v>
@@ -4417,7 +4528,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4428,7 +4539,7 @@
         <v>41</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>40</v>
@@ -4440,18 +4551,20 @@
         <v>51</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="N31" s="2"/>
+        <v>219</v>
+      </c>
+      <c r="N31" t="s" s="2">
+        <v>220</v>
+      </c>
       <c r="O31" t="s" s="2">
         <v>40</v>
       </c>
@@ -4472,7 +4585,7 @@
         <v>40</v>
       </c>
       <c r="V31" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W31" t="s" s="2">
         <v>40</v>
@@ -4498,37 +4611,33 @@
       <c r="AD31" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AE31" t="s" s="2">
+      <c r="AE31" s="2"/>
+      <c r="AF31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG31" s="2"/>
+      <c r="AH31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK31" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="AL31" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="AM31" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="AF31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AH31" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI31" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="AJ31" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK31" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL31" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="AM31" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" hidden="true">
-      <c r="A32" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4536,28 +4645,28 @@
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F32" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H32" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I32" t="s" s="2">
         <v>40</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>202</v>
+        <v>224</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>203</v>
+        <v>225</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -4584,13 +4693,11 @@
         <v>41</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X32" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="X32" s="2"/>
       <c r="Y32" t="s" s="2">
-        <v>40</v>
+        <v>226</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>40</v>
@@ -4608,7 +4715,7 @@
         <v>40</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>41</v>
@@ -4623,54 +4730,52 @@
         <v>40</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>40</v>
+        <v>223</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>40</v>
+        <v>227</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>204</v>
+        <v>40</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>40</v>
+        <v>228</v>
       </c>
     </row>
-    <row r="33" hidden="true">
+    <row r="33">
       <c r="A33" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H33" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I33" t="s" s="2">
         <v>40</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>91</v>
+        <v>230</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>206</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>93</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>40</v>
@@ -4695,13 +4800,11 @@
         <v>41</v>
       </c>
       <c r="W33" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X33" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="X33" s="2"/>
       <c r="Y33" t="s" s="2">
-        <v>40</v>
+        <v>232</v>
       </c>
       <c r="Z33" t="s" s="2">
         <v>40</v>
@@ -4719,13 +4822,13 @@
         <v>40</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH33" t="s" s="2">
         <v>40</v>
@@ -4734,53 +4837,53 @@
         <v>40</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>40</v>
+        <v>229</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>40</v>
+        <v>233</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>204</v>
+        <v>234</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>40</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>208</v>
+        <v>40</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G34" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I34" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="I34" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J34" t="s" s="2">
-        <v>90</v>
+        <v>143</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>103</v>
+        <v>236</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>209</v>
+        <v>237</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>93</v>
+        <v>238</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
@@ -4806,13 +4909,13 @@
         <v>41</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>40</v>
+        <v>239</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>40</v>
@@ -4830,13 +4933,13 @@
         <v>40</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH34" t="s" s="2">
         <v>40</v>
@@ -4848,18 +4951,18 @@
         <v>40</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>40</v>
+        <v>240</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>87</v>
+        <v>241</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>40</v>
+        <v>242</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -4882,15 +4985,17 @@
         <v>51</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>143</v>
+        <v>244</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="M35" s="2"/>
+        <v>246</v>
+      </c>
+      <c r="M35" t="s" s="2">
+        <v>247</v>
+      </c>
       <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
         <v>40</v>
@@ -4915,11 +5020,13 @@
         <v>41</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>213</v>
-      </c>
-      <c r="X35" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="X35" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Y35" t="s" s="2">
-        <v>235</v>
+        <v>40</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>40</v>
@@ -4937,7 +5044,7 @@
         <v>40</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>41</v>
@@ -4946,7 +5053,7 @@
         <v>50</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>236</v>
+        <v>40</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>40</v>
@@ -4955,18 +5062,18 @@
         <v>40</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>40</v>
+        <v>248</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>40</v>
+        <v>250</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -4977,7 +5084,7 @@
         <v>41</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>40</v>
@@ -4989,15 +5096,17 @@
         <v>51</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="M36" s="2"/>
+        <v>254</v>
+      </c>
+      <c r="M36" t="s" s="2">
+        <v>255</v>
+      </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
         <v>40</v>
@@ -5046,16 +5155,16 @@
         <v>40</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>236</v>
+        <v>40</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>40</v>
@@ -5067,15 +5176,15 @@
         <v>40</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>222</v>
+        <v>256</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>40</v>
+        <v>257</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5086,7 +5195,7 @@
         <v>41</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>40</v>
@@ -5098,17 +5207,15 @@
         <v>51</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>143</v>
+        <v>259</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>243</v>
+        <v>260</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>245</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
         <v>40</v>
@@ -5133,11 +5240,13 @@
         <v>41</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>146</v>
-      </c>
-      <c r="X37" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="X37" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Y37" t="s" s="2">
-        <v>246</v>
+        <v>40</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>40</v>
@@ -5155,19 +5264,19 @@
         <v>40</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>40</v>
@@ -5176,7 +5285,7 @@
         <v>40</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>40</v>
@@ -5184,7 +5293,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5210,10 +5319,10 @@
         <v>52</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>202</v>
+        <v>162</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>203</v>
+        <v>163</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5237,7 +5346,7 @@
         <v>40</v>
       </c>
       <c r="V38" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="W38" t="s" s="2">
         <v>40</v>
@@ -5263,11 +5372,15 @@
       <c r="AD38" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AE38" s="2"/>
+      <c r="AE38" t="s" s="2">
+        <v>264</v>
+      </c>
       <c r="AF38" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AG38" s="2"/>
+      <c r="AG38" t="s" s="2">
+        <v>50</v>
+      </c>
       <c r="AH38" t="s" s="2">
         <v>40</v>
       </c>
@@ -5281,7 +5394,7 @@
         <v>40</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>204</v>
+        <v>164</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>40</v>
@@ -5289,7 +5402,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>249</v>
+        <v>265</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5318,7 +5431,7 @@
         <v>91</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>206</v>
+        <v>166</v>
       </c>
       <c r="M39" t="s" s="2">
         <v>93</v>
@@ -5344,7 +5457,7 @@
         <v>40</v>
       </c>
       <c r="V39" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="W39" t="s" s="2">
         <v>40</v>
@@ -5359,20 +5472,26 @@
         <v>40</v>
       </c>
       <c r="AA39" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="AB39" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="AB39" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="AC39" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD39" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="AE39" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="AE39" t="s" s="2">
+        <v>265</v>
+      </c>
       <c r="AF39" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AG39" s="2"/>
+      <c r="AG39" t="s" s="2">
+        <v>42</v>
+      </c>
       <c r="AH39" t="s" s="2">
         <v>40</v>
       </c>
@@ -5386,7 +5505,7 @@
         <v>40</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>204</v>
+        <v>164</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>40</v>
@@ -5394,13 +5513,11 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="B40" t="s" s="2">
-        <v>250</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>40</v>
+        <v>267</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
@@ -5413,19 +5530,23 @@
         <v>40</v>
       </c>
       <c r="H40" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I40" t="s" s="2">
         <v>40</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="K40" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="K40" t="s" s="2">
+        <v>103</v>
+      </c>
       <c r="L40" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="M40" s="2"/>
+        <v>268</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>93</v>
+      </c>
       <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
         <v>40</v>
@@ -5447,7 +5568,7 @@
         <v>40</v>
       </c>
       <c r="V40" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="W40" t="s" s="2">
         <v>40</v>
@@ -5474,7 +5595,7 @@
         <v>40</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>41</v>
@@ -5495,7 +5616,7 @@
         <v>40</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>40</v>
@@ -5503,11 +5624,9 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="B41" t="s" s="2">
-        <v>253</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
         <v>40</v>
       </c>
@@ -5516,7 +5635,7 @@
         <v>41</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>40</v>
@@ -5525,14 +5644,16 @@
         <v>40</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="K41" s="2"/>
+        <v>143</v>
+      </c>
+      <c r="K41" t="s" s="2">
+        <v>270</v>
+      </c>
       <c r="L41" t="s" s="2">
-        <v>255</v>
+        <v>271</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -5556,16 +5677,16 @@
         <v>40</v>
       </c>
       <c r="V41" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="W41" t="s" s="2">
-        <v>40</v>
+        <v>272</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>40</v>
+        <v>273</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>40</v>
+        <v>274</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>40</v>
@@ -5583,16 +5704,16 @@
         <v>40</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH41" t="s" s="2">
-        <v>40</v>
+        <v>275</v>
       </c>
       <c r="AI41" t="s" s="2">
         <v>40</v>
@@ -5601,10 +5722,10 @@
         <v>40</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>40</v>
+        <v>149</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>40</v>
@@ -5612,11 +5733,9 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="B42" t="s" s="2">
-        <v>256</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
         <v>40</v>
       </c>
@@ -5625,7 +5744,7 @@
         <v>41</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>40</v>
@@ -5634,14 +5753,16 @@
         <v>40</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="K42" s="2"/>
+        <v>278</v>
+      </c>
+      <c r="K42" t="s" s="2">
+        <v>279</v>
+      </c>
       <c r="L42" t="s" s="2">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -5665,7 +5786,7 @@
         <v>40</v>
       </c>
       <c r="V42" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="W42" t="s" s="2">
         <v>40</v>
@@ -5692,7 +5813,7 @@
         <v>40</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>249</v>
+        <v>277</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>41</v>
@@ -5701,7 +5822,7 @@
         <v>42</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>40</v>
+        <v>275</v>
       </c>
       <c r="AI42" t="s" s="2">
         <v>40</v>
@@ -5713,7 +5834,7 @@
         <v>40</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>40</v>
+        <v>281</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>40</v>
@@ -5721,7 +5842,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>259</v>
+        <v>282</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -5744,20 +5865,18 @@
         <v>51</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>261</v>
+        <v>283</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>262</v>
+        <v>284</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>263</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>264</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>40</v>
       </c>
@@ -5778,7 +5897,7 @@
         <v>40</v>
       </c>
       <c r="V43" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="W43" t="s" s="2">
         <v>40</v>
@@ -5804,25 +5923,29 @@
       <c r="AD43" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AE43" s="2"/>
+      <c r="AE43" t="s" s="2">
+        <v>282</v>
+      </c>
       <c r="AF43" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AG43" s="2"/>
+      <c r="AG43" t="s" s="2">
+        <v>42</v>
+      </c>
       <c r="AH43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>40</v>
+        <v>286</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>265</v>
+        <v>40</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>266</v>
+        <v>287</v>
       </c>
       <c r="AM43" t="s" s="2">
         <v>40</v>
@@ -5830,7 +5953,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>267</v>
+        <v>288</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -5850,23 +5973,19 @@
         <v>40</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>268</v>
+        <v>52</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>269</v>
+        <v>162</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>272</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
         <v>40</v>
       </c>
@@ -5887,7 +6006,7 @@
         <v>40</v>
       </c>
       <c r="V44" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="W44" t="s" s="2">
         <v>40</v>
@@ -5913,11 +6032,15 @@
       <c r="AD44" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AE44" s="2"/>
+      <c r="AE44" t="s" s="2">
+        <v>288</v>
+      </c>
       <c r="AF44" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AG44" s="2"/>
+      <c r="AG44" t="s" s="2">
+        <v>50</v>
+      </c>
       <c r="AH44" t="s" s="2">
         <v>40</v>
       </c>
@@ -5928,10 +6051,10 @@
         <v>40</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>273</v>
+        <v>40</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>274</v>
+        <v>164</v>
       </c>
       <c r="AM44" t="s" s="2">
         <v>40</v>
@@ -5939,18 +6062,18 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>40</v>
@@ -5959,18 +6082,20 @@
         <v>40</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>268</v>
+        <v>90</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>276</v>
+        <v>91</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="M45" s="2"/>
+        <v>166</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>93</v>
+      </c>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
         <v>40</v>
@@ -6019,35 +6144,1335 @@
         <v>40</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG45" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH45" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI45" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ45" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK45" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL45" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="AM45" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" hidden="true">
+      <c r="A46" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F46" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H46" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="I46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J46" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="K46" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="L46" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="M46" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="N46" s="2"/>
+      <c r="O46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P46" s="2"/>
+      <c r="Q46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V46" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE46" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="AF46" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG46" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL46" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AM46" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" hidden="true">
+      <c r="A47" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F47" t="s" s="2">
         <v>50</v>
       </c>
-      <c r="AH45" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI45" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ45" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK45" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="AL45" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="AM45" t="s" s="2">
+      <c r="G47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I47" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J47" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="K47" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="L47" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P47" s="2"/>
+      <c r="Q47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V47" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W47" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="X47" s="2"/>
+      <c r="Y47" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="Z47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE47" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="AF47" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG47" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH47" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="AI47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL47" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="AM47" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" hidden="true">
+      <c r="A48" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F48" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I48" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J48" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="K48" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="L48" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P48" s="2"/>
+      <c r="Q48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V48" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE48" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="AF48" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG48" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH48" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="AI48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL48" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="AM48" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" hidden="true">
+      <c r="A49" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F49" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I49" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J49" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="K49" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="L49" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="M49" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="N49" s="2"/>
+      <c r="O49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P49" s="2"/>
+      <c r="Q49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V49" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W49" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="X49" s="2"/>
+      <c r="Y49" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="Z49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE49" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="AF49" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG49" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL49" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="AM49" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" hidden="true">
+      <c r="A50" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="B50" s="2"/>
+      <c r="C50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F50" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J50" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K50" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P50" s="2"/>
+      <c r="Q50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE50" s="2"/>
+      <c r="AF50" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG50" s="2"/>
+      <c r="AH50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL50" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="AM50" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" hidden="true">
+      <c r="A51" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F51" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J51" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="K51" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="L51" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="M51" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="N51" s="2"/>
+      <c r="O51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P51" s="2"/>
+      <c r="Q51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA51" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AB51" s="2"/>
+      <c r="AC51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD51" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AE51" s="2"/>
+      <c r="AF51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG51" s="2"/>
+      <c r="AH51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL51" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="AM51" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" hidden="true">
+      <c r="A52" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="B52" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="C52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F52" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J52" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="K52" s="2"/>
+      <c r="L52" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P52" s="2"/>
+      <c r="Q52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE52" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="AF52" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG52" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM52" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" hidden="true">
+      <c r="A53" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="B53" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="C53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F53" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J53" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="K53" s="2"/>
+      <c r="L53" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P53" s="2"/>
+      <c r="Q53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE53" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="AF53" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG53" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM53" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" hidden="true">
+      <c r="A54" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="B54" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="C54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F54" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J54" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="K54" s="2"/>
+      <c r="L54" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P54" s="2"/>
+      <c r="Q54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM54" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" hidden="true">
+      <c r="A55" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F55" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I55" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J55" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="K55" t="s" s="2">
+        <v>169</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="M55" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="N55" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="O55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P55" s="2"/>
+      <c r="Q55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE55" s="2"/>
+      <c r="AF55" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG55" s="2"/>
+      <c r="AH55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK55" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="AL55" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="AM55" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" hidden="true">
+      <c r="A56" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F56" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I56" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J56" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="K56" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="L56" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="N56" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="O56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P56" s="2"/>
+      <c r="Q56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE56" s="2"/>
+      <c r="AF56" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG56" s="2"/>
+      <c r="AH56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK56" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="AL56" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="AM56" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" hidden="true">
+      <c r="A57" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F57" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I57" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J57" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="K57" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="L57" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P57" s="2"/>
+      <c r="Q57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V57" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE57" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="AF57" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG57" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK57" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="AL57" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="AM57" t="s" s="2">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM45">
+  <autoFilter ref="A1:AM57">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -6057,7 +7482,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI44">
+  <conditionalFormatting sqref="A2:AI56">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>